<commit_message>
UjianNomor 2 Ujian JC Data Science
</commit_message>
<xml_diff>
--- a/2.xlsx
+++ b/2.xlsx
@@ -14,69 +14,33 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="21">
-  <si>
-    <t>P</t>
-  </si>
-  <si>
-    <t>u</t>
-  </si>
-  <si>
-    <t>r</t>
-  </si>
-  <si>
-    <t>w</t>
-  </si>
-  <si>
-    <t>a</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+  <si>
+    <t>k</t>
+  </si>
+  <si>
+    <t>o</t>
   </si>
   <si>
     <t>d</t>
   </si>
   <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>t</t>
+  </si>
+  <si>
     <t>h</t>
   </si>
   <si>
-    <t>i</t>
-  </si>
-  <si>
-    <t>k</t>
-  </si>
-  <si>
-    <t>S</t>
-  </si>
-  <si>
-    <t>t</t>
-  </si>
-  <si>
-    <t>p</t>
-  </si>
-  <si>
     <t>n</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>o</t>
-  </si>
-  <si>
-    <t>g</t>
-  </si>
-  <si>
-    <t>c</t>
-  </si>
-  <si>
-    <t>l</t>
-  </si>
-  <si>
-    <t>@</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>D</t>
   </si>
 </sst>
 </file>
@@ -408,18 +372,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -427,7 +391,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -438,7 +402,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -446,96 +410,10 @@
         <v>7</v>
       </c>
       <c r="C4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
         <v>8</v>
-      </c>
-      <c r="D4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" t="s">
-        <v>2</v>
-      </c>
-      <c r="E5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" t="s">
-        <v>5</v>
-      </c>
-      <c r="F6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" t="s">
-        <v>15</v>
-      </c>
-      <c r="F7" t="s">
-        <v>9</v>
-      </c>
-      <c r="G7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="A8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" t="s">
-        <v>17</v>
-      </c>
-      <c r="E8" t="s">
-        <v>18</v>
-      </c>
-      <c r="F8" t="s">
-        <v>19</v>
-      </c>
-      <c r="G8" t="s">
-        <v>9</v>
-      </c>
-      <c r="H8" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ujian Nomor 2 Ujian JC Data Science
</commit_message>
<xml_diff>
--- a/2.xlsx
+++ b/2.xlsx
@@ -14,33 +14,69 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="21">
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>u</t>
+  </si>
+  <si>
+    <t>r</t>
+  </si>
+  <si>
+    <t>w</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>h</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
   <si>
     <t>k</t>
   </si>
   <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>t</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
     <t>o</t>
   </si>
   <si>
-    <t>d</t>
-  </si>
-  <si>
-    <t>e</t>
-  </si>
-  <si>
-    <t>p</t>
-  </si>
-  <si>
-    <t>y</t>
-  </si>
-  <si>
-    <t>t</t>
-  </si>
-  <si>
-    <t>h</t>
-  </si>
-  <si>
-    <t>n</t>
+    <t>g</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>l</t>
+  </si>
+  <si>
+    <t>@</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>D</t>
   </si>
 </sst>
 </file>
@@ -372,18 +408,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -391,7 +427,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -402,7 +438,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -410,10 +446,96 @@
         <v>7</v>
       </c>
       <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" t="s">
         <v>1</v>
       </c>
-      <c r="D4" t="s">
-        <v>8</v>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" t="s">
+        <v>9</v>
+      </c>
+      <c r="H8" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>